<commit_message>
final auto gen constant
</commit_message>
<xml_diff>
--- a/src/main/resources/api_master/ApiMaster.xlsx
+++ b/src/main/resources/api_master/ApiMaster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="api_config" sheetId="2" r:id="rId1"/>
@@ -111,7 +111,7 @@
     <t>BASE_URL</t>
   </si>
   <si>
-    <t>/golf-cms/api/booking/abc</t>
+    <t>/golf-cms/api/e-invoice/abc</t>
   </si>
   <si>
     <t>GET</t>
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>

</xml_diff>

<commit_message>
auto gen api registry and create template voucher check
</commit_message>
<xml_diff>
--- a/src/main/resources/api_master/ApiMaster.xlsx
+++ b/src/main/resources/api_master/ApiMaster.xlsx
@@ -111,7 +111,7 @@
     <t>BASE_URL</t>
   </si>
   <si>
-    <t>/golf-cms/api/e-invoice/abc</t>
+    <t>/golf-cms/api/booking/abc</t>
   </si>
   <si>
     <t>GET</t>
@@ -132,7 +132,7 @@
     <t>testABC</t>
   </si>
   <si>
-    <t>abc_id</t>
+    <t>abc_case_id</t>
   </si>
   <si>
     <t>defTest</t>
@@ -1519,7 +1519,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3"/>

</xml_diff>

<commit_message>
update flow voucher green
</commit_message>
<xml_diff>
--- a/src/main/resources/api_master/ApiMaster.xlsx
+++ b/src/main/resources/api_master/ApiMaster.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>module</t>
   </si>
@@ -120,6 +120,57 @@
   </si>
   <si>
     <t>quote_fee_voucher_case_id</t>
+  </si>
+  <si>
+    <t>booking/checkin</t>
+  </si>
+  <si>
+    <t>CheckInBagPlayer1VoucherTest</t>
+  </si>
+  <si>
+    <t>checkInBagData</t>
+  </si>
+  <si>
+    <t>/golf-cms/api/booking/check-in</t>
+  </si>
+  <si>
+    <t>input_excel_file/booking/CheckIn.xlsx</t>
+  </si>
+  <si>
+    <t>Check_In_Bag_Player1_VC</t>
+  </si>
+  <si>
+    <t>input_json_file/booking/check_in/</t>
+  </si>
+  <si>
+    <t>testCheckInBag</t>
+  </si>
+  <si>
+    <t>check_in_bag_player1_voucher_case_id</t>
+  </si>
+  <si>
+    <t>booking/edit_booking</t>
+  </si>
+  <si>
+    <t>EditBooking1PlayerVoucherTest</t>
+  </si>
+  <si>
+    <t>EditBookingData</t>
+  </si>
+  <si>
+    <t>/golf-cms/api/booking/update</t>
+  </si>
+  <si>
+    <t>Edit_Booking_1_Player_VC</t>
+  </si>
+  <si>
+    <t>input_json_file/booking/edit_booking/</t>
+  </si>
+  <si>
+    <t>testEditBooking</t>
+  </si>
+  <si>
+    <t>edit_booking_1player_voucher_case_id</t>
   </si>
 </sst>
 </file>
@@ -1303,24 +1354,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="20.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.8571428571429" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.8571428571429" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.8571428571429" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.4285714285714" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5714285714286" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.1428571428571" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.4285714285714" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.7142857142857" style="1" customWidth="1"/>
-    <col min="8" max="10" width="20.1428571428571" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="10" width="20.1428571428571" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.8571428571429" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1428571428571" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
@@ -1438,6 +1490,82 @@
         <v>30</v>
       </c>
     </row>
+    <row r="4" ht="45" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" ht="45" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>